<commit_message>
change calculation for heuristic 4
</commit_message>
<xml_diff>
--- a/rush_hour_analysis.xlsx
+++ b/rush_hour_analysis.xlsx
@@ -489,7 +489,7 @@
         <v>1174</v>
       </c>
       <c r="G2" t="n">
-        <v>2.26</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="3">
@@ -570,7 +570,7 @@
         <v>415</v>
       </c>
       <c r="G5" t="n">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="6">
@@ -594,10 +594,10 @@
         <v>8</v>
       </c>
       <c r="F6" t="n">
-        <v>1174</v>
+        <v>54</v>
       </c>
       <c r="G6" t="n">
-        <v>2.15</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -624,7 +624,7 @@
         <v>1146</v>
       </c>
       <c r="G7" t="n">
-        <v>2.23</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="8">
@@ -651,7 +651,7 @@
         <v>1146</v>
       </c>
       <c r="G8" t="n">
-        <v>2.23</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="9">
@@ -678,7 +678,7 @@
         <v>424</v>
       </c>
       <c r="G9" t="n">
-        <v>0.72</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -702,10 +702,10 @@
         <v>8</v>
       </c>
       <c r="F10" t="n">
-        <v>1174</v>
+        <v>1082</v>
       </c>
       <c r="G10" t="n">
-        <v>2.29</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="11">
@@ -837,10 +837,10 @@
         <v>5</v>
       </c>
       <c r="F15" t="n">
-        <v>309</v>
+        <v>13</v>
       </c>
       <c r="G15" t="n">
-        <v>0.37</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="16">
@@ -867,7 +867,7 @@
         <v>131</v>
       </c>
       <c r="G16" t="n">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="17">
@@ -945,10 +945,10 @@
         <v>5</v>
       </c>
       <c r="F19" t="n">
-        <v>309</v>
+        <v>99</v>
       </c>
       <c r="G19" t="n">
-        <v>0.38</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="20">
@@ -975,7 +975,7 @@
         <v>1140</v>
       </c>
       <c r="G20" t="n">
-        <v>1.67</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="21">
@@ -1002,7 +1002,7 @@
         <v>255</v>
       </c>
       <c r="G21" t="n">
-        <v>0.32</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="22">
@@ -1029,7 +1029,7 @@
         <v>255</v>
       </c>
       <c r="G22" t="n">
-        <v>0.3</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="23">
@@ -1056,7 +1056,7 @@
         <v>255</v>
       </c>
       <c r="G23" t="n">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="24">
@@ -1080,10 +1080,10 @@
         <v>15</v>
       </c>
       <c r="F24" t="n">
-        <v>1140</v>
+        <v>219</v>
       </c>
       <c r="G24" t="n">
-        <v>1.58</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="25">
@@ -1110,7 +1110,7 @@
         <v>1082</v>
       </c>
       <c r="G25" t="n">
-        <v>1.59</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="26">
@@ -1137,7 +1137,7 @@
         <v>1082</v>
       </c>
       <c r="G26" t="n">
-        <v>1.6</v>
+        <v>1.61</v>
       </c>
     </row>
     <row r="27">
@@ -1188,10 +1188,10 @@
         <v>15</v>
       </c>
       <c r="F28" t="n">
-        <v>1140</v>
+        <v>1022</v>
       </c>
       <c r="G28" t="n">
-        <v>1.71</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="29">
@@ -1218,7 +1218,7 @@
         <v>499</v>
       </c>
       <c r="G29" t="n">
-        <v>1.07</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="30">
@@ -1272,7 +1272,7 @@
         <v>10</v>
       </c>
       <c r="G31" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="32">
@@ -1299,7 +1299,7 @@
         <v>10</v>
       </c>
       <c r="G32" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="33">
@@ -1323,10 +1323,10 @@
         <v>4</v>
       </c>
       <c r="F33" t="n">
-        <v>499</v>
+        <v>10</v>
       </c>
       <c r="G33" t="n">
-        <v>1.07</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="34">
@@ -1380,7 +1380,7 @@
         <v>127</v>
       </c>
       <c r="G35" t="n">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="36">
@@ -1431,10 +1431,10 @@
         <v>4</v>
       </c>
       <c r="F37" t="n">
-        <v>499</v>
+        <v>127</v>
       </c>
       <c r="G37" t="n">
-        <v>1.05</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="38">
@@ -1461,7 +1461,7 @@
         <v>1491</v>
       </c>
       <c r="G38" t="n">
-        <v>2.44</v>
+        <v>2.71</v>
       </c>
     </row>
     <row r="39">
@@ -1488,7 +1488,7 @@
         <v>400</v>
       </c>
       <c r="G39" t="n">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="40">
@@ -1566,10 +1566,10 @@
         <v>15</v>
       </c>
       <c r="F42" t="n">
-        <v>1491</v>
+        <v>258</v>
       </c>
       <c r="G42" t="n">
-        <v>2.21</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="43">
@@ -1596,7 +1596,7 @@
         <v>1128</v>
       </c>
       <c r="G43" t="n">
-        <v>1.75</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="44">
@@ -1623,7 +1623,7 @@
         <v>1128</v>
       </c>
       <c r="G44" t="n">
-        <v>1.74</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="45">
@@ -1650,7 +1650,7 @@
         <v>788</v>
       </c>
       <c r="G45" t="n">
-        <v>1.16</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="46">
@@ -1674,10 +1674,10 @@
         <v>15</v>
       </c>
       <c r="F46" t="n">
-        <v>1491</v>
+        <v>989</v>
       </c>
       <c r="G46" t="n">
-        <v>2.47</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="47">
@@ -1809,10 +1809,10 @@
         <v>4</v>
       </c>
       <c r="F51" t="n">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="G51" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1839,7 +1839,7 @@
         <v>32</v>
       </c>
       <c r="G52" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="53">
@@ -1866,7 +1866,7 @@
         <v>32</v>
       </c>
       <c r="G53" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="54">
@@ -1917,10 +1917,10 @@
         <v>4</v>
       </c>
       <c r="F55" t="n">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="G55" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="56">
@@ -2001,7 +2001,7 @@
         <v>7</v>
       </c>
       <c r="G58" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="59">
@@ -2028,7 +2028,7 @@
         <v>7</v>
       </c>
       <c r="G59" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -2052,10 +2052,10 @@
         <v>3</v>
       </c>
       <c r="F60" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G60" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -2160,10 +2160,10 @@
         <v>3</v>
       </c>
       <c r="F64" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G64" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="65">
@@ -2295,10 +2295,10 @@
         <v>4</v>
       </c>
       <c r="F69" t="n">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G69" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -2403,10 +2403,10 @@
         <v>4</v>
       </c>
       <c r="F73" t="n">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="G73" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="74">
@@ -2433,7 +2433,7 @@
         <v>1237</v>
       </c>
       <c r="G74" t="n">
-        <v>1.67</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="75">
@@ -2460,7 +2460,7 @@
         <v>530</v>
       </c>
       <c r="G75" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="76">
@@ -2487,7 +2487,7 @@
         <v>530</v>
       </c>
       <c r="G76" t="n">
-        <v>0.54</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="77">
@@ -2535,13 +2535,13 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F78" t="n">
-        <v>1237</v>
+        <v>563</v>
       </c>
       <c r="G78" t="n">
-        <v>1.56</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="79">
@@ -2568,7 +2568,7 @@
         <v>958</v>
       </c>
       <c r="G79" t="n">
-        <v>1.19</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="80">
@@ -2595,7 +2595,7 @@
         <v>958</v>
       </c>
       <c r="G80" t="n">
-        <v>1.17</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="81">
@@ -2622,7 +2622,7 @@
         <v>603</v>
       </c>
       <c r="G81" t="n">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="82">
@@ -2646,10 +2646,10 @@
         <v>16</v>
       </c>
       <c r="F82" t="n">
-        <v>1237</v>
+        <v>833</v>
       </c>
       <c r="G82" t="n">
-        <v>1.71</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="83">
@@ -2703,7 +2703,7 @@
         <v>12</v>
       </c>
       <c r="G84" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="85">
@@ -2778,13 +2778,13 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F87" t="n">
-        <v>816</v>
+        <v>18</v>
       </c>
       <c r="G87" t="n">
-        <v>1.83</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="88">
@@ -2889,10 +2889,10 @@
         <v>4</v>
       </c>
       <c r="F91" t="n">
-        <v>816</v>
+        <v>138</v>
       </c>
       <c r="G91" t="n">
-        <v>1.76</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="92">
@@ -2919,7 +2919,7 @@
         <v>616</v>
       </c>
       <c r="G92" t="n">
-        <v>1.15</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="93">
@@ -3000,7 +3000,7 @@
         <v>25</v>
       </c>
       <c r="G95" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="96">
@@ -3021,13 +3021,13 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F96" t="n">
-        <v>616</v>
+        <v>25</v>
       </c>
       <c r="G96" t="n">
-        <v>1.18</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="97">
@@ -3132,10 +3132,10 @@
         <v>4</v>
       </c>
       <c r="F100" t="n">
-        <v>616</v>
+        <v>101</v>
       </c>
       <c r="G100" t="n">
-        <v>1.17</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="101">
@@ -3162,7 +3162,7 @@
         <v>74</v>
       </c>
       <c r="G101" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="102">
@@ -3267,10 +3267,10 @@
         <v>3</v>
       </c>
       <c r="F105" t="n">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="G105" t="n">
-        <v>0.11</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="106">
@@ -3324,7 +3324,7 @@
         <v>74</v>
       </c>
       <c r="G107" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="108">
@@ -3375,10 +3375,10 @@
         <v>3</v>
       </c>
       <c r="F109" t="n">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G109" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="110">
@@ -3405,7 +3405,7 @@
         <v>448</v>
       </c>
       <c r="G110" t="n">
-        <v>0.75</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="111">
@@ -3510,10 +3510,10 @@
         <v>5</v>
       </c>
       <c r="F114" t="n">
-        <v>448</v>
+        <v>10</v>
       </c>
       <c r="G114" t="n">
-        <v>0.75</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="115">
@@ -3618,10 +3618,10 @@
         <v>5</v>
       </c>
       <c r="F118" t="n">
-        <v>448</v>
+        <v>77</v>
       </c>
       <c r="G118" t="n">
-        <v>0.75</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="119">
@@ -3648,7 +3648,7 @@
         <v>288</v>
       </c>
       <c r="G119" t="n">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="120">
@@ -3753,10 +3753,10 @@
         <v>4</v>
       </c>
       <c r="F123" t="n">
-        <v>288</v>
+        <v>10</v>
       </c>
       <c r="G123" t="n">
-        <v>0.39</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="124">
@@ -3783,7 +3783,7 @@
         <v>77</v>
       </c>
       <c r="G124" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="125">
@@ -3861,10 +3861,10 @@
         <v>4</v>
       </c>
       <c r="F127" t="n">
-        <v>288</v>
+        <v>77</v>
       </c>
       <c r="G127" t="n">
-        <v>0.39</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="128">
@@ -3891,7 +3891,7 @@
         <v>189</v>
       </c>
       <c r="G128" t="n">
-        <v>0.28</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="129">
@@ -3918,7 +3918,7 @@
         <v>11</v>
       </c>
       <c r="G129" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="130">
@@ -3972,7 +3972,7 @@
         <v>11</v>
       </c>
       <c r="G131" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="132">
@@ -3996,10 +3996,10 @@
         <v>4</v>
       </c>
       <c r="F132" t="n">
-        <v>189</v>
+        <v>10</v>
       </c>
       <c r="G132" t="n">
-        <v>0.27</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="133">
@@ -4080,7 +4080,7 @@
         <v>11</v>
       </c>
       <c r="G135" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="136">
@@ -4104,10 +4104,10 @@
         <v>4</v>
       </c>
       <c r="F136" t="n">
-        <v>189</v>
+        <v>30</v>
       </c>
       <c r="G136" t="n">
-        <v>0.27</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="137">
@@ -4134,7 +4134,7 @@
         <v>136</v>
       </c>
       <c r="G137" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="138">
@@ -4239,10 +4239,10 @@
         <v>5</v>
       </c>
       <c r="F141" t="n">
-        <v>136</v>
+        <v>28</v>
       </c>
       <c r="G141" t="n">
-        <v>0.11</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="142">
@@ -4296,7 +4296,7 @@
         <v>80</v>
       </c>
       <c r="G143" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="144">
@@ -4347,10 +4347,10 @@
         <v>5</v>
       </c>
       <c r="F145" t="n">
-        <v>136</v>
+        <v>80</v>
       </c>
       <c r="G145" t="n">
-        <v>0.11</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="146">
@@ -4482,10 +4482,10 @@
         <v>2</v>
       </c>
       <c r="F150" t="n">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="G150" t="n">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="151">
@@ -4590,10 +4590,10 @@
         <v>2</v>
       </c>
       <c r="F154" t="n">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="G154" t="n">
-        <v>0.2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="155">
@@ -4620,7 +4620,7 @@
         <v>1142</v>
       </c>
       <c r="G155" t="n">
-        <v>2.2</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="156">
@@ -4674,7 +4674,7 @@
         <v>113</v>
       </c>
       <c r="G157" t="n">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="158">
@@ -4722,13 +4722,13 @@
         </is>
       </c>
       <c r="E159" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F159" t="n">
-        <v>1142</v>
+        <v>43</v>
       </c>
       <c r="G159" t="n">
-        <v>2.13</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="160">
@@ -4755,7 +4755,7 @@
         <v>656</v>
       </c>
       <c r="G160" t="n">
-        <v>1.13</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="161">
@@ -4782,7 +4782,7 @@
         <v>656</v>
       </c>
       <c r="G161" t="n">
-        <v>1.15</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="162">
@@ -4809,7 +4809,7 @@
         <v>113</v>
       </c>
       <c r="G162" t="n">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="163">
@@ -4833,10 +4833,10 @@
         <v>6</v>
       </c>
       <c r="F163" t="n">
-        <v>1142</v>
+        <v>568</v>
       </c>
       <c r="G163" t="n">
-        <v>2.21</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="164">
@@ -4863,7 +4863,7 @@
         <v>185</v>
       </c>
       <c r="G164" t="n">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="165">
@@ -4968,10 +4968,10 @@
         <v>3</v>
       </c>
       <c r="F168" t="n">
-        <v>185</v>
+        <v>7</v>
       </c>
       <c r="G168" t="n">
-        <v>0.27</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="169">
@@ -5025,7 +5025,7 @@
         <v>31</v>
       </c>
       <c r="G170" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="171">
@@ -5076,10 +5076,10 @@
         <v>3</v>
       </c>
       <c r="F172" t="n">
-        <v>185</v>
+        <v>28</v>
       </c>
       <c r="G172" t="n">
-        <v>0.26</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="173">
@@ -5211,10 +5211,10 @@
         <v>3</v>
       </c>
       <c r="F177" t="n">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="G177" t="n">
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="178">
@@ -5319,10 +5319,10 @@
         <v>3</v>
       </c>
       <c r="F181" t="n">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="G181" t="n">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="182">
@@ -5454,10 +5454,10 @@
         <v>4</v>
       </c>
       <c r="F186" t="n">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="G186" t="n">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="187">
@@ -5484,7 +5484,7 @@
         <v>81</v>
       </c>
       <c r="G187" t="n">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="188">
@@ -5562,10 +5562,10 @@
         <v>4</v>
       </c>
       <c r="F190" t="n">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="G190" t="n">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="191">
@@ -5619,7 +5619,7 @@
         <v>7</v>
       </c>
       <c r="G192" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -5673,7 +5673,7 @@
         <v>7</v>
       </c>
       <c r="G194" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -5697,10 +5697,10 @@
         <v>4</v>
       </c>
       <c r="F195" t="n">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="G195" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="196">
@@ -5805,10 +5805,10 @@
         <v>4</v>
       </c>
       <c r="F199" t="n">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="G199" t="n">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="200">
@@ -5835,7 +5835,7 @@
         <v>1474</v>
       </c>
       <c r="G200" t="n">
-        <v>3.23</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="201">
@@ -5862,7 +5862,7 @@
         <v>68</v>
       </c>
       <c r="G201" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="202">
@@ -5937,13 +5937,13 @@
         </is>
       </c>
       <c r="E204" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F204" t="n">
-        <v>1474</v>
+        <v>27</v>
       </c>
       <c r="G204" t="n">
-        <v>3.12</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="205">
@@ -6048,10 +6048,10 @@
         <v>6</v>
       </c>
       <c r="F208" t="n">
-        <v>1474</v>
+        <v>374</v>
       </c>
       <c r="G208" t="n">
-        <v>3.25</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="209">
@@ -6183,10 +6183,10 @@
         <v>3</v>
       </c>
       <c r="F213" t="n">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="G213" t="n">
-        <v>0.12</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="214">
@@ -6291,10 +6291,10 @@
         <v>3</v>
       </c>
       <c r="F217" t="n">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="G217" t="n">
-        <v>0.12</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="218">
@@ -6321,7 +6321,7 @@
         <v>239</v>
       </c>
       <c r="G218" t="n">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="219">
@@ -6426,10 +6426,10 @@
         <v>3</v>
       </c>
       <c r="F222" t="n">
-        <v>239</v>
+        <v>13</v>
       </c>
       <c r="G222" t="n">
-        <v>0.43</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="223">
@@ -6534,10 +6534,10 @@
         <v>3</v>
       </c>
       <c r="F226" t="n">
-        <v>239</v>
+        <v>67</v>
       </c>
       <c r="G226" t="n">
-        <v>0.43</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="227">
@@ -6564,7 +6564,7 @@
         <v>607</v>
       </c>
       <c r="G227" t="n">
-        <v>1.1</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="228">
@@ -6669,10 +6669,10 @@
         <v>5</v>
       </c>
       <c r="F231" t="n">
-        <v>607</v>
+        <v>15</v>
       </c>
       <c r="G231" t="n">
-        <v>1.09</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="232">
@@ -6777,10 +6777,10 @@
         <v>5</v>
       </c>
       <c r="F235" t="n">
-        <v>607</v>
+        <v>423</v>
       </c>
       <c r="G235" t="n">
-        <v>1.11</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="236">
@@ -6807,7 +6807,7 @@
         <v>449</v>
       </c>
       <c r="G236" t="n">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="237">
@@ -6912,10 +6912,10 @@
         <v>5</v>
       </c>
       <c r="F240" t="n">
-        <v>449</v>
+        <v>9</v>
       </c>
       <c r="G240" t="n">
-        <v>0.72</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="241">
@@ -6942,7 +6942,7 @@
         <v>145</v>
       </c>
       <c r="G241" t="n">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="242">
@@ -7020,10 +7020,10 @@
         <v>5</v>
       </c>
       <c r="F244" t="n">
-        <v>449</v>
+        <v>88</v>
       </c>
       <c r="G244" t="n">
-        <v>0.7</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="245">
@@ -7155,10 +7155,10 @@
         <v>3</v>
       </c>
       <c r="F249" t="n">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="G249" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="250">
@@ -7263,7 +7263,7 @@
         <v>3</v>
       </c>
       <c r="F253" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G253" t="n">
         <v>0.02</v>
@@ -7293,7 +7293,7 @@
         <v>5729</v>
       </c>
       <c r="G254" t="n">
-        <v>26.11</v>
+        <v>26.25</v>
       </c>
     </row>
     <row r="255">
@@ -7347,7 +7347,7 @@
         <v>1933</v>
       </c>
       <c r="G256" t="n">
-        <v>4.18</v>
+        <v>4.06</v>
       </c>
     </row>
     <row r="257">
@@ -7374,7 +7374,7 @@
         <v>1933</v>
       </c>
       <c r="G257" t="n">
-        <v>4.18</v>
+        <v>4.13</v>
       </c>
     </row>
     <row r="258">
@@ -7395,13 +7395,13 @@
         </is>
       </c>
       <c r="E258" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F258" t="n">
-        <v>5729</v>
+        <v>1385</v>
       </c>
       <c r="G258" t="n">
-        <v>21.12</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="259">
@@ -7428,7 +7428,7 @@
         <v>3920</v>
       </c>
       <c r="G259" t="n">
-        <v>14.08</v>
+        <v>13.93</v>
       </c>
     </row>
     <row r="260">
@@ -7455,7 +7455,7 @@
         <v>3920</v>
       </c>
       <c r="G260" t="n">
-        <v>14.11</v>
+        <v>14.02</v>
       </c>
     </row>
     <row r="261">
@@ -7482,7 +7482,7 @@
         <v>1944</v>
       </c>
       <c r="G261" t="n">
-        <v>4.68</v>
+        <v>4.62</v>
       </c>
     </row>
     <row r="262">
@@ -7506,10 +7506,10 @@
         <v>16</v>
       </c>
       <c r="F262" t="n">
-        <v>5729</v>
+        <v>3002</v>
       </c>
       <c r="G262" t="n">
-        <v>27.89</v>
+        <v>8.970000000000001</v>
       </c>
     </row>
     <row r="263">
@@ -7641,10 +7641,10 @@
         <v>5</v>
       </c>
       <c r="F267" t="n">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="G267" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="268">
@@ -7671,7 +7671,7 @@
         <v>65</v>
       </c>
       <c r="G268" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="269">
@@ -7749,10 +7749,10 @@
         <v>5</v>
       </c>
       <c r="F271" t="n">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="G271" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="272">
@@ -7884,10 +7884,10 @@
         <v>3</v>
       </c>
       <c r="F276" t="n">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="G276" t="n">
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="277">
@@ -7941,7 +7941,7 @@
         <v>41</v>
       </c>
       <c r="G278" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="279">
@@ -7992,10 +7992,10 @@
         <v>3</v>
       </c>
       <c r="F280" t="n">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="G280" t="n">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="281">
@@ -8022,7 +8022,7 @@
         <v>5891</v>
       </c>
       <c r="G281" t="n">
-        <v>33.66</v>
+        <v>33.27</v>
       </c>
     </row>
     <row r="282">
@@ -8049,7 +8049,7 @@
         <v>798</v>
       </c>
       <c r="G282" t="n">
-        <v>1.33</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="283">
@@ -8076,7 +8076,7 @@
         <v>798</v>
       </c>
       <c r="G283" t="n">
-        <v>1.26</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="284">
@@ -8103,7 +8103,7 @@
         <v>798</v>
       </c>
       <c r="G284" t="n">
-        <v>1.28</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="285">
@@ -8124,13 +8124,13 @@
         </is>
       </c>
       <c r="E285" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F285" t="n">
-        <v>5891</v>
+        <v>700</v>
       </c>
       <c r="G285" t="n">
-        <v>28.56</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="286">
@@ -8157,7 +8157,7 @@
         <v>2372</v>
       </c>
       <c r="G286" t="n">
-        <v>8.029999999999999</v>
+        <v>7.81</v>
       </c>
     </row>
     <row r="287">
@@ -8184,7 +8184,7 @@
         <v>2372</v>
       </c>
       <c r="G287" t="n">
-        <v>8.029999999999999</v>
+        <v>7.88</v>
       </c>
     </row>
     <row r="288">
@@ -8235,10 +8235,10 @@
         <v>12</v>
       </c>
       <c r="F289" t="n">
-        <v>5891</v>
+        <v>1916</v>
       </c>
       <c r="G289" t="n">
-        <v>34.6</v>
+        <v>5.77</v>
       </c>
     </row>
     <row r="290">
@@ -8265,7 +8265,7 @@
         <v>27</v>
       </c>
       <c r="G290" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="291">
@@ -8319,7 +8319,7 @@
         <v>10</v>
       </c>
       <c r="G292" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="293">
@@ -8370,10 +8370,10 @@
         <v>3</v>
       </c>
       <c r="F294" t="n">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="G294" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="295">
@@ -8478,10 +8478,10 @@
         <v>3</v>
       </c>
       <c r="F298" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G298" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="299">
@@ -8508,7 +8508,7 @@
         <v>351</v>
       </c>
       <c r="G299" t="n">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="300">
@@ -8613,10 +8613,10 @@
         <v>4</v>
       </c>
       <c r="F303" t="n">
-        <v>351</v>
+        <v>23</v>
       </c>
       <c r="G303" t="n">
-        <v>0.44</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="304">
@@ -8721,10 +8721,10 @@
         <v>4</v>
       </c>
       <c r="F307" t="n">
-        <v>351</v>
+        <v>79</v>
       </c>
       <c r="G307" t="n">
-        <v>0.44</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="308">
@@ -8751,7 +8751,7 @@
         <v>209</v>
       </c>
       <c r="G308" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="309">
@@ -8856,10 +8856,10 @@
         <v>4</v>
       </c>
       <c r="F312" t="n">
-        <v>209</v>
+        <v>10</v>
       </c>
       <c r="G312" t="n">
-        <v>0.23</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="313">
@@ -8964,10 +8964,10 @@
         <v>4</v>
       </c>
       <c r="F316" t="n">
-        <v>209</v>
+        <v>34</v>
       </c>
       <c r="G316" t="n">
-        <v>0.23</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="317">
@@ -8994,7 +8994,7 @@
         <v>653</v>
       </c>
       <c r="G317" t="n">
-        <v>1.12</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="318">
@@ -9075,7 +9075,7 @@
         <v>43</v>
       </c>
       <c r="G320" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="321">
@@ -9096,13 +9096,13 @@
         </is>
       </c>
       <c r="E321" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F321" t="n">
-        <v>653</v>
+        <v>43</v>
       </c>
       <c r="G321" t="n">
-        <v>1.12</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="322">
@@ -9129,7 +9129,7 @@
         <v>237</v>
       </c>
       <c r="G322" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="323">
@@ -9156,7 +9156,7 @@
         <v>237</v>
       </c>
       <c r="G323" t="n">
-        <v>0.34</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="324">
@@ -9207,10 +9207,10 @@
         <v>5</v>
       </c>
       <c r="F325" t="n">
-        <v>653</v>
+        <v>226</v>
       </c>
       <c r="G325" t="n">
-        <v>1.12</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="326">
@@ -9237,7 +9237,7 @@
         <v>5223</v>
       </c>
       <c r="G326" t="n">
-        <v>22.57</v>
+        <v>22.45</v>
       </c>
     </row>
     <row r="327">
@@ -9264,7 +9264,7 @@
         <v>4237</v>
       </c>
       <c r="G327" t="n">
-        <v>15.58</v>
+        <v>15.31</v>
       </c>
     </row>
     <row r="328">
@@ -9291,7 +9291,7 @@
         <v>4237</v>
       </c>
       <c r="G328" t="n">
-        <v>15.55</v>
+        <v>15.44</v>
       </c>
     </row>
     <row r="329">
@@ -9318,7 +9318,7 @@
         <v>4237</v>
       </c>
       <c r="G329" t="n">
-        <v>15.69</v>
+        <v>15.48</v>
       </c>
     </row>
     <row r="330">
@@ -9339,13 +9339,13 @@
         </is>
       </c>
       <c r="E330" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F330" t="n">
-        <v>5223</v>
+        <v>4184</v>
       </c>
       <c r="G330" t="n">
-        <v>18.62</v>
+        <v>14.77</v>
       </c>
     </row>
     <row r="331">
@@ -9372,7 +9372,7 @@
         <v>4893</v>
       </c>
       <c r="G331" t="n">
-        <v>20.92</v>
+        <v>20.72</v>
       </c>
     </row>
     <row r="332">
@@ -9399,7 +9399,7 @@
         <v>4893</v>
       </c>
       <c r="G332" t="n">
-        <v>21</v>
+        <v>20.83</v>
       </c>
     </row>
     <row r="333">
@@ -9426,7 +9426,7 @@
         <v>4303</v>
       </c>
       <c r="G333" t="n">
-        <v>18.18</v>
+        <v>17.84</v>
       </c>
     </row>
     <row r="334">
@@ -9450,10 +9450,10 @@
         <v>20</v>
       </c>
       <c r="F334" t="n">
-        <v>5223</v>
+        <v>4566</v>
       </c>
       <c r="G334" t="n">
-        <v>23.39</v>
+        <v>18.91</v>
       </c>
     </row>
     <row r="335">
@@ -9585,10 +9585,10 @@
         <v>2</v>
       </c>
       <c r="F339" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="G339" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="340">
@@ -9693,10 +9693,10 @@
         <v>2</v>
       </c>
       <c r="F343" t="n">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="G343" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="344">
@@ -9723,7 +9723,7 @@
         <v>456</v>
       </c>
       <c r="G344" t="n">
-        <v>0.76</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="345">
@@ -9750,7 +9750,7 @@
         <v>12</v>
       </c>
       <c r="G345" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="346">
@@ -9804,7 +9804,7 @@
         <v>12</v>
       </c>
       <c r="G347" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="348">
@@ -9828,10 +9828,10 @@
         <v>4</v>
       </c>
       <c r="F348" t="n">
-        <v>456</v>
+        <v>12</v>
       </c>
       <c r="G348" t="n">
-        <v>0.77</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="349">
@@ -9885,7 +9885,7 @@
         <v>93</v>
       </c>
       <c r="G350" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="351">
@@ -9912,7 +9912,7 @@
         <v>12</v>
       </c>
       <c r="G351" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="352">
@@ -9936,10 +9936,10 @@
         <v>4</v>
       </c>
       <c r="F352" t="n">
-        <v>456</v>
+        <v>91</v>
       </c>
       <c r="G352" t="n">
-        <v>0.76</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="353">
@@ -9966,7 +9966,7 @@
         <v>364</v>
       </c>
       <c r="G353" t="n">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="354">
@@ -10068,13 +10068,13 @@
         </is>
       </c>
       <c r="E357" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F357" t="n">
-        <v>364</v>
+        <v>145</v>
       </c>
       <c r="G357" t="n">
-        <v>0.35</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="358">
@@ -10128,7 +10128,7 @@
         <v>249</v>
       </c>
       <c r="G359" t="n">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="360">
@@ -10179,10 +10179,10 @@
         <v>9</v>
       </c>
       <c r="F361" t="n">
-        <v>364</v>
+        <v>226</v>
       </c>
       <c r="G361" t="n">
-        <v>0.36</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="362">
@@ -10209,7 +10209,7 @@
         <v>1218</v>
       </c>
       <c r="G362" t="n">
-        <v>2.26</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="363">
@@ -10236,7 +10236,7 @@
         <v>92</v>
       </c>
       <c r="G363" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="364">
@@ -10314,10 +10314,10 @@
         <v>7</v>
       </c>
       <c r="F366" t="n">
-        <v>1218</v>
+        <v>90</v>
       </c>
       <c r="G366" t="n">
-        <v>2.21</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="367">
@@ -10344,7 +10344,7 @@
         <v>732</v>
       </c>
       <c r="G367" t="n">
-        <v>1.17</v>
+        <v>1.16</v>
       </c>
     </row>
     <row r="368">
@@ -10371,7 +10371,7 @@
         <v>732</v>
       </c>
       <c r="G368" t="n">
-        <v>1.18</v>
+        <v>1.15</v>
       </c>
     </row>
     <row r="369">
@@ -10398,7 +10398,7 @@
         <v>92</v>
       </c>
       <c r="G369" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="370">
@@ -10422,10 +10422,10 @@
         <v>7</v>
       </c>
       <c r="F370" t="n">
-        <v>1218</v>
+        <v>718</v>
       </c>
       <c r="G370" t="n">
-        <v>2.28</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="371">
@@ -10557,10 +10557,10 @@
         <v>5</v>
       </c>
       <c r="F375" t="n">
-        <v>241</v>
+        <v>68</v>
       </c>
       <c r="G375" t="n">
-        <v>0.27</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="376">
@@ -10587,7 +10587,7 @@
         <v>193</v>
       </c>
       <c r="G376" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="377">
@@ -10614,7 +10614,7 @@
         <v>193</v>
       </c>
       <c r="G377" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="378">
@@ -10665,10 +10665,10 @@
         <v>5</v>
       </c>
       <c r="F379" t="n">
-        <v>241</v>
+        <v>193</v>
       </c>
       <c r="G379" t="n">
-        <v>0.27</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="380">
@@ -10800,10 +10800,10 @@
         <v>4</v>
       </c>
       <c r="F384" t="n">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="G384" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="385">
@@ -10830,7 +10830,7 @@
         <v>49</v>
       </c>
       <c r="G385" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="386">
@@ -10857,7 +10857,7 @@
         <v>49</v>
       </c>
       <c r="G386" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="387">
@@ -10908,10 +10908,10 @@
         <v>4</v>
       </c>
       <c r="F388" t="n">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="G388" t="n">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="389">
@@ -11286,10 +11286,10 @@
         <v>2</v>
       </c>
       <c r="F402" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G402" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="403">
@@ -11394,10 +11394,10 @@
         <v>2</v>
       </c>
       <c r="F406" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G406" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="407">
@@ -11451,7 +11451,7 @@
         <v>15</v>
       </c>
       <c r="G408" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="409">
@@ -11478,7 +11478,7 @@
         <v>15</v>
       </c>
       <c r="G409" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="410">
@@ -11529,10 +11529,10 @@
         <v>4</v>
       </c>
       <c r="F411" t="n">
-        <v>235</v>
+        <v>12</v>
       </c>
       <c r="G411" t="n">
-        <v>0.3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="412">
@@ -11637,10 +11637,10 @@
         <v>4</v>
       </c>
       <c r="F415" t="n">
-        <v>235</v>
+        <v>51</v>
       </c>
       <c r="G415" t="n">
-        <v>0.29</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="416">
@@ -11667,7 +11667,7 @@
         <v>228</v>
       </c>
       <c r="G416" t="n">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="417">
@@ -11772,10 +11772,10 @@
         <v>8</v>
       </c>
       <c r="F420" t="n">
-        <v>228</v>
+        <v>62</v>
       </c>
       <c r="G420" t="n">
-        <v>0.22</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="421">
@@ -11856,7 +11856,7 @@
         <v>83</v>
       </c>
       <c r="G423" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="424">
@@ -11880,10 +11880,10 @@
         <v>8</v>
       </c>
       <c r="F424" t="n">
-        <v>228</v>
+        <v>144</v>
       </c>
       <c r="G424" t="n">
-        <v>0.22</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="425">
@@ -12015,10 +12015,10 @@
         <v>3</v>
       </c>
       <c r="F429" t="n">
-        <v>176</v>
+        <v>11</v>
       </c>
       <c r="G429" t="n">
-        <v>0.22</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="430">
@@ -12123,10 +12123,10 @@
         <v>3</v>
       </c>
       <c r="F433" t="n">
-        <v>176</v>
+        <v>32</v>
       </c>
       <c r="G433" t="n">
-        <v>0.22</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="434">
@@ -12153,7 +12153,7 @@
         <v>4309</v>
       </c>
       <c r="G434" t="n">
-        <v>19.66</v>
+        <v>19.58</v>
       </c>
     </row>
     <row r="435">
@@ -12180,7 +12180,7 @@
         <v>1152</v>
       </c>
       <c r="G435" t="n">
-        <v>2.61</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="436">
@@ -12207,7 +12207,7 @@
         <v>1152</v>
       </c>
       <c r="G436" t="n">
-        <v>2.62</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="437">
@@ -12234,7 +12234,7 @@
         <v>1152</v>
       </c>
       <c r="G437" t="n">
-        <v>2.66</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="438">
@@ -12255,13 +12255,13 @@
         </is>
       </c>
       <c r="E438" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F438" t="n">
-        <v>4309</v>
+        <v>1152</v>
       </c>
       <c r="G438" t="n">
-        <v>16.13</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="439">
@@ -12288,7 +12288,7 @@
         <v>2888</v>
       </c>
       <c r="G439" t="n">
-        <v>10.3</v>
+        <v>10.17</v>
       </c>
     </row>
     <row r="440">
@@ -12315,7 +12315,7 @@
         <v>2888</v>
       </c>
       <c r="G440" t="n">
-        <v>10.29</v>
+        <v>10.2</v>
       </c>
     </row>
     <row r="441">
@@ -12342,7 +12342,7 @@
         <v>2114</v>
       </c>
       <c r="G441" t="n">
-        <v>5.91</v>
+        <v>5.83</v>
       </c>
     </row>
     <row r="442">
@@ -12366,10 +12366,10 @@
         <v>16</v>
       </c>
       <c r="F442" t="n">
-        <v>4309</v>
+        <v>2888</v>
       </c>
       <c r="G442" t="n">
-        <v>20.73</v>
+        <v>10.11</v>
       </c>
     </row>
     <row r="443">
@@ -12396,7 +12396,7 @@
         <v>190</v>
       </c>
       <c r="G443" t="n">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="444">
@@ -12501,10 +12501,10 @@
         <v>7</v>
       </c>
       <c r="F447" t="n">
-        <v>190</v>
+        <v>59</v>
       </c>
       <c r="G447" t="n">
-        <v>0.17</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="448">
@@ -12531,7 +12531,7 @@
         <v>170</v>
       </c>
       <c r="G448" t="n">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="449">
@@ -12609,10 +12609,10 @@
         <v>7</v>
       </c>
       <c r="F451" t="n">
-        <v>190</v>
+        <v>156</v>
       </c>
       <c r="G451" t="n">
-        <v>0.17</v>
+        <v>0.14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add search analysis excel file
</commit_message>
<xml_diff>
--- a/rush_hour_analysis.xlsx
+++ b/rush_hour_analysis.xlsx
@@ -651,7 +651,7 @@
         <v>7</v>
       </c>
       <c r="G8" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -732,7 +732,7 @@
         <v>1836</v>
       </c>
       <c r="G11" t="n">
-        <v>3.2</v>
+        <v>3.38</v>
       </c>
     </row>
     <row r="12">
@@ -759,7 +759,7 @@
         <v>116</v>
       </c>
       <c r="G12" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="13">
@@ -786,7 +786,7 @@
         <v>116</v>
       </c>
       <c r="G13" t="n">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="14">
@@ -813,7 +813,7 @@
         <v>116</v>
       </c>
       <c r="G14" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="15">
@@ -867,7 +867,7 @@
         <v>591</v>
       </c>
       <c r="G16" t="n">
-        <v>0.85</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="17">
@@ -894,7 +894,7 @@
         <v>591</v>
       </c>
       <c r="G17" t="n">
-        <v>0.87</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="18">
@@ -921,7 +921,7 @@
         <v>143</v>
       </c>
       <c r="G18" t="n">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="19">
@@ -948,7 +948,7 @@
         <v>367</v>
       </c>
       <c r="G19" t="n">
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="20">
@@ -975,7 +975,7 @@
         <v>5240</v>
       </c>
       <c r="G20" t="n">
-        <v>6.61</v>
+        <v>6.53</v>
       </c>
     </row>
     <row r="21">
@@ -1002,7 +1002,7 @@
         <v>2910</v>
       </c>
       <c r="G21" t="n">
-        <v>3.66</v>
+        <v>3.68</v>
       </c>
     </row>
     <row r="22">
@@ -1029,7 +1029,7 @@
         <v>2910</v>
       </c>
       <c r="G22" t="n">
-        <v>3.66</v>
+        <v>3.62</v>
       </c>
     </row>
     <row r="23">
@@ -1056,7 +1056,7 @@
         <v>2910</v>
       </c>
       <c r="G23" t="n">
-        <v>3.5</v>
+        <v>3.56</v>
       </c>
     </row>
     <row r="24">
@@ -1083,7 +1083,7 @@
         <v>774</v>
       </c>
       <c r="G24" t="n">
-        <v>1.01</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="25">
@@ -1110,7 +1110,7 @@
         <v>4855</v>
       </c>
       <c r="G25" t="n">
-        <v>6.07</v>
+        <v>6.32</v>
       </c>
     </row>
     <row r="26">
@@ -1137,7 +1137,7 @@
         <v>4855</v>
       </c>
       <c r="G26" t="n">
-        <v>6.31</v>
+        <v>6.51</v>
       </c>
     </row>
     <row r="27">
@@ -1164,7 +1164,7 @@
         <v>2342</v>
       </c>
       <c r="G27" t="n">
-        <v>3.38</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="28">
@@ -1191,7 +1191,7 @@
         <v>4386</v>
       </c>
       <c r="G28" t="n">
-        <v>5.8</v>
+        <v>5.79</v>
       </c>
     </row>
     <row r="29">
@@ -1218,7 +1218,7 @@
         <v>156</v>
       </c>
       <c r="G29" t="n">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="30">
@@ -1299,7 +1299,7 @@
         <v>156</v>
       </c>
       <c r="G32" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="33">
@@ -1326,7 +1326,7 @@
         <v>156</v>
       </c>
       <c r="G33" t="n">
-        <v>0.13</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="34">
@@ -1461,7 +1461,7 @@
         <v>353</v>
       </c>
       <c r="G38" t="n">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="39">
@@ -1488,7 +1488,7 @@
         <v>353</v>
       </c>
       <c r="G39" t="n">
-        <v>0.29</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="40">
@@ -1542,7 +1542,7 @@
         <v>353</v>
       </c>
       <c r="G41" t="n">
-        <v>0.28</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="42">
@@ -1569,7 +1569,7 @@
         <v>353</v>
       </c>
       <c r="G42" t="n">
-        <v>0.29</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="43">
@@ -1677,7 +1677,7 @@
         <v>353</v>
       </c>
       <c r="G46" t="n">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="47">
@@ -1758,7 +1758,7 @@
         <v>561</v>
       </c>
       <c r="G49" t="n">
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="50">
@@ -1785,7 +1785,7 @@
         <v>561</v>
       </c>
       <c r="G50" t="n">
-        <v>0.42</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="51">
@@ -1812,7 +1812,7 @@
         <v>535</v>
       </c>
       <c r="G51" t="n">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="52">
@@ -1839,7 +1839,7 @@
         <v>647</v>
       </c>
       <c r="G52" t="n">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="53">
@@ -1893,7 +1893,7 @@
         <v>556</v>
       </c>
       <c r="G54" t="n">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="55">

</xml_diff>